<commit_message>
test find store and invalid login completed
</commit_message>
<xml_diff>
--- a/com.optimum/src/test/resources/test_data.xlsx
+++ b/com.optimum/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.optimum\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3961AF0D-4DE6-40D9-A498-0FD0C60CF01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEFF827-F822-49F5-B4EC-C159CBDE13D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3BBA78DA-4EC1-4C55-9720-CDE8982C35FD}"/>
+    <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{3BBA78DA-4EC1-4C55-9720-CDE8982C35FD}"/>
   </bookViews>
   <sheets>
     <sheet name="doCheckAvailability" sheetId="1" r:id="rId1"/>
+    <sheet name="doFindStoreLocator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Street Address</t>
   </si>
@@ -49,16 +50,50 @@
   </si>
   <si>
     <t xml:space="preserve">15 preston st </t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Bridgeport, CT</t>
+  </si>
+  <si>
+    <t>Lake Charles, LA</t>
+  </si>
+  <si>
+    <t>Brooklyn, NY</t>
+  </si>
+  <si>
+    <t>Abilene, TX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +116,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75F7995-F680-42B3-9948-5B5C4C7D94E7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -446,4 +487,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553BF877-B208-4399-BB67-FE112DD4A466}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>